<commit_message>
add dark mode , company search by name , improve css
</commit_message>
<xml_diff>
--- a/public/plats.xlsx
+++ b/public/plats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>TechAviv</t>
   </si>
@@ -218,6 +218,18 @@
   </si>
   <si>
     <t>https://www.barakl.co.il/</t>
+  </si>
+  <si>
+    <t>https://www.jsjobs.co.il/positions/</t>
+  </si>
+  <si>
+    <t>Jumpstart</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/hila-results-inc/jobs/</t>
+  </si>
+  <si>
+    <t>Hila Results inc.</t>
   </si>
 </sst>
 </file>
@@ -570,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -610,10 +622,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -621,10 +633,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -632,10 +644,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -643,10 +655,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -654,10 +666,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -665,10 +677,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -676,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -687,10 +699,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -698,10 +710,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -709,10 +721,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -720,10 +732,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -731,10 +743,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -742,10 +754,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -753,10 +765,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -764,10 +776,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -775,10 +787,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -786,10 +798,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -797,10 +809,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -808,10 +820,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -819,10 +831,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -830,10 +842,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -841,10 +853,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -852,10 +864,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -863,10 +875,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -874,10 +886,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -885,10 +897,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -896,10 +908,10 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -907,10 +919,10 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -918,10 +930,10 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,10 +941,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -940,10 +952,10 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -951,51 +963,74 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:C33">
-    <sortCondition ref="B1"/>
+  <sortState ref="A3:C36">
+    <sortCondition ref="B19"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C31" r:id="rId1"/>
-    <hyperlink ref="C30" r:id="rId2"/>
-    <hyperlink ref="C21" r:id="rId3"/>
+    <hyperlink ref="C34" r:id="rId1"/>
+    <hyperlink ref="C33" r:id="rId2"/>
+    <hyperlink ref="C23" r:id="rId3"/>
     <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="C4" r:id="rId5"/>
-    <hyperlink ref="C16" r:id="rId6"/>
-    <hyperlink ref="C23" r:id="rId7"/>
-    <hyperlink ref="C8" r:id="rId8"/>
-    <hyperlink ref="C9" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C29" r:id="rId12"/>
-    <hyperlink ref="C13" r:id="rId13"/>
-    <hyperlink ref="C33" r:id="rId14"/>
-    <hyperlink ref="C15" r:id="rId15"/>
-    <hyperlink ref="C32" r:id="rId16"/>
-    <hyperlink ref="C14" r:id="rId17"/>
-    <hyperlink ref="C27" r:id="rId18"/>
-    <hyperlink ref="C28" r:id="rId19"/>
-    <hyperlink ref="C7" r:id="rId20"/>
-    <hyperlink ref="C6" r:id="rId21"/>
-    <hyperlink ref="C10" r:id="rId22"/>
-    <hyperlink ref="C19" r:id="rId23"/>
-    <hyperlink ref="C20" r:id="rId24"/>
-    <hyperlink ref="C22" r:id="rId25"/>
-    <hyperlink ref="C25" r:id="rId26"/>
-    <hyperlink ref="C24" r:id="rId27"/>
-    <hyperlink ref="C5" r:id="rId28"/>
-    <hyperlink ref="C3" r:id="rId29"/>
-    <hyperlink ref="C18" r:id="rId30"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C17" r:id="rId6"/>
+    <hyperlink ref="C26" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C32" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C36" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C35" r:id="rId16"/>
+    <hyperlink ref="C15" r:id="rId17"/>
+    <hyperlink ref="C30" r:id="rId18"/>
+    <hyperlink ref="C31" r:id="rId19"/>
+    <hyperlink ref="C8" r:id="rId20"/>
+    <hyperlink ref="C7" r:id="rId21"/>
+    <hyperlink ref="C11" r:id="rId22"/>
+    <hyperlink ref="C21" r:id="rId23"/>
+    <hyperlink ref="C22" r:id="rId24"/>
+    <hyperlink ref="C24" r:id="rId25"/>
+    <hyperlink ref="C28" r:id="rId26"/>
+    <hyperlink ref="C27" r:id="rId27"/>
+    <hyperlink ref="C6" r:id="rId28"/>
+    <hyperlink ref="C4" r:id="rId29"/>
+    <hyperlink ref="C20" r:id="rId30"/>
     <hyperlink ref="C1" r:id="rId31"/>
-    <hyperlink ref="C17" r:id="rId32"/>
-    <hyperlink ref="C26" r:id="rId33"/>
-    <hyperlink ref="C34" r:id="rId34"/>
+    <hyperlink ref="C19" r:id="rId32"/>
+    <hyperlink ref="C29" r:id="rId33"/>
+    <hyperlink ref="C3" r:id="rId34"/>
+    <hyperlink ref="C18" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates and code impronment
</commit_message>
<xml_diff>
--- a/public/plats.xlsx
+++ b/public/plats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>TechAviv</t>
   </si>
@@ -230,6 +230,18 @@
   </si>
   <si>
     <t>Hila Results inc.</t>
+  </si>
+  <si>
+    <t>ZipRecruiter </t>
+  </si>
+  <si>
+    <t>https://www.ziprecruiter.co.uk/</t>
+  </si>
+  <si>
+    <t>goozali</t>
+  </si>
+  <si>
+    <t>https://goozali.com/</t>
   </si>
 </sst>
 </file>
@@ -582,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -611,10 +623,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -622,10 +634,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -776,10 +788,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -787,10 +799,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -798,10 +810,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,10 +821,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -820,10 +832,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -831,10 +843,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -842,10 +854,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -853,10 +865,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -864,10 +876,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -875,10 +887,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -886,10 +898,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -897,10 +909,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -908,10 +920,10 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -919,10 +931,10 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -930,10 +942,10 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -941,10 +953,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -952,10 +964,10 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -963,10 +975,10 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -974,10 +986,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -985,52 +997,76 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A3:C36">
+  <sortState ref="A1:C38">
     <sortCondition ref="B19"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C34" r:id="rId1"/>
-    <hyperlink ref="C33" r:id="rId2"/>
-    <hyperlink ref="C23" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="C35" r:id="rId1"/>
+    <hyperlink ref="C34" r:id="rId2"/>
+    <hyperlink ref="C24" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
     <hyperlink ref="C5" r:id="rId5"/>
-    <hyperlink ref="C17" r:id="rId6"/>
-    <hyperlink ref="C26" r:id="rId7"/>
+    <hyperlink ref="C18" r:id="rId6"/>
+    <hyperlink ref="C27" r:id="rId7"/>
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C12" r:id="rId10"/>
     <hyperlink ref="C13" r:id="rId11"/>
-    <hyperlink ref="C32" r:id="rId12"/>
+    <hyperlink ref="C33" r:id="rId12"/>
     <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C36" r:id="rId14"/>
+    <hyperlink ref="C37" r:id="rId14"/>
     <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C35" r:id="rId16"/>
+    <hyperlink ref="C36" r:id="rId16"/>
     <hyperlink ref="C15" r:id="rId17"/>
-    <hyperlink ref="C30" r:id="rId18"/>
-    <hyperlink ref="C31" r:id="rId19"/>
+    <hyperlink ref="C31" r:id="rId18"/>
+    <hyperlink ref="C32" r:id="rId19"/>
     <hyperlink ref="C8" r:id="rId20"/>
     <hyperlink ref="C7" r:id="rId21"/>
     <hyperlink ref="C11" r:id="rId22"/>
-    <hyperlink ref="C21" r:id="rId23"/>
-    <hyperlink ref="C22" r:id="rId24"/>
-    <hyperlink ref="C24" r:id="rId25"/>
-    <hyperlink ref="C28" r:id="rId26"/>
-    <hyperlink ref="C27" r:id="rId27"/>
+    <hyperlink ref="C22" r:id="rId23"/>
+    <hyperlink ref="C23" r:id="rId24"/>
+    <hyperlink ref="C25" r:id="rId25"/>
+    <hyperlink ref="C29" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
     <hyperlink ref="C6" r:id="rId28"/>
     <hyperlink ref="C4" r:id="rId29"/>
-    <hyperlink ref="C20" r:id="rId30"/>
+    <hyperlink ref="C21" r:id="rId30"/>
     <hyperlink ref="C1" r:id="rId31"/>
-    <hyperlink ref="C19" r:id="rId32"/>
-    <hyperlink ref="C29" r:id="rId33"/>
-    <hyperlink ref="C3" r:id="rId34"/>
-    <hyperlink ref="C18" r:id="rId35"/>
+    <hyperlink ref="C20" r:id="rId32"/>
+    <hyperlink ref="C30" r:id="rId33"/>
+    <hyperlink ref="C2" r:id="rId34"/>
+    <hyperlink ref="C19" r:id="rId35"/>
+    <hyperlink ref="C38" r:id="rId36"/>
+    <hyperlink ref="C17" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>